<commit_message>
Added TableOfContents and Subject-Local-Place fields
</commit_message>
<xml_diff>
--- a/digitalcollections-standard-metadata.xlsx
+++ b/digitalcollections-standard-metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Lehigh\Work From Home\Spreadsheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Lehigh\Work From Home\Spreadsheet\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00702635-7444-4320-97B0-CA39C163E560}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70EBA08A-DB02-4ECD-8EAB-8AF7757ED315}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Islandora Metadata Template" sheetId="1" r:id="rId1"/>
@@ -216,7 +216,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{A45955F0-C447-4E97-A7BA-BD50D6CFDEEA}">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{A45955F0-C447-4E97-A7BA-BD50D6CFDEEA}">
       <text>
         <r>
           <rPr>
@@ -242,7 +242,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{454DE92F-D709-4465-BBD9-0A87F9FE3884}">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{454DE92F-D709-4465-BBD9-0A87F9FE3884}">
       <text>
         <r>
           <rPr>
@@ -268,7 +268,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{B54B678A-3085-4E00-B156-EEE7F291535C}">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{B54B678A-3085-4E00-B156-EEE7F291535C}">
       <text>
         <r>
           <rPr>
@@ -293,7 +293,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{63A938D5-DD9F-4C28-85B7-862F01C2557B}">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{63A938D5-DD9F-4C28-85B7-862F01C2557B}">
       <text>
         <r>
           <rPr>
@@ -319,7 +319,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{F3FC3F32-7AD5-4AD5-BC96-E284BC31D639}">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{F3FC3F32-7AD5-4AD5-BC96-E284BC31D639}">
       <text>
         <r>
           <rPr>
@@ -346,7 +346,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{C8C7F5BA-7F77-486D-89C1-EE8841EBF865}">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{C8C7F5BA-7F77-486D-89C1-EE8841EBF865}">
       <text>
         <r>
           <rPr>
@@ -372,7 +372,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{E3B509DE-43E9-44B5-BDEC-98F9565127F8}">
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{E3B509DE-43E9-44B5-BDEC-98F9565127F8}">
       <text>
         <r>
           <rPr>
@@ -396,7 +396,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{E2CC8CA8-D47F-4EEC-A37F-5713BAB9E324}">
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{E2CC8CA8-D47F-4EEC-A37F-5713BAB9E324}">
       <text>
         <r>
           <rPr>
@@ -420,7 +420,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{091FF495-4462-4CC1-8F23-39AEEA05BB0A}">
+    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{091FF495-4462-4CC1-8F23-39AEEA05BB0A}">
       <text>
         <r>
           <rPr>
@@ -446,7 +446,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{E08F8DEB-76A8-4E0E-966F-F84105839B5D}">
+    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{E08F8DEB-76A8-4E0E-966F-F84105839B5D}">
       <text>
         <r>
           <rPr>
@@ -470,7 +470,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{C37A58A6-F5F3-40F1-A828-7C18B781422F}">
+    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{C37A58A6-F5F3-40F1-A828-7C18B781422F}">
       <text>
         <r>
           <rPr>
@@ -496,7 +496,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{3991E12B-3A71-4A97-B3B5-1180C0193E47}">
+    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{3991E12B-3A71-4A97-B3B5-1180C0193E47}">
       <text>
         <r>
           <rPr>
@@ -522,7 +522,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{85E6D484-5A90-45DD-9A06-ACAEA4E36301}">
+    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{85E6D484-5A90-45DD-9A06-ACAEA4E36301}">
       <text>
         <r>
           <rPr>
@@ -548,7 +548,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{F6F51BBE-97C7-4474-9B6A-5F28B5E6742F}">
+    <comment ref="X1" authorId="0" shapeId="0" xr:uid="{F6F51BBE-97C7-4474-9B6A-5F28B5E6742F}">
       <text>
         <r>
           <rPr>
@@ -573,7 +573,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0" shapeId="0" xr:uid="{4BBD92AC-9B74-421C-B77E-49175DBE1818}">
+    <comment ref="Y1" authorId="0" shapeId="0" xr:uid="{4BBD92AC-9B74-421C-B77E-49175DBE1818}">
       <text>
         <r>
           <rPr>
@@ -599,7 +599,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="0" shapeId="0" xr:uid="{A13F7FB5-2D79-4361-A957-990F73831417}">
+    <comment ref="Z1" authorId="0" shapeId="0" xr:uid="{A13F7FB5-2D79-4361-A957-990F73831417}">
       <text>
         <r>
           <rPr>
@@ -624,7 +624,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="0" shapeId="0" xr:uid="{6FFEBC39-3422-4FA0-98D2-223893A185AA}">
+    <comment ref="AA1" authorId="0" shapeId="0" xr:uid="{6FFEBC39-3422-4FA0-98D2-223893A185AA}">
       <text>
         <r>
           <rPr>
@@ -650,7 +650,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA1" authorId="0" shapeId="0" xr:uid="{5D40D71D-7BB4-4B93-99E1-B2FD752A62E9}">
+    <comment ref="AB1" authorId="0" shapeId="0" xr:uid="{5D40D71D-7BB4-4B93-99E1-B2FD752A62E9}">
       <text>
         <r>
           <rPr>
@@ -679,7 +679,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB1" authorId="0" shapeId="0" xr:uid="{FC850D2C-B335-4894-B732-C94221F61B96}">
+    <comment ref="AC1" authorId="0" shapeId="0" xr:uid="{FC850D2C-B335-4894-B732-C94221F61B96}">
       <text>
         <r>
           <rPr>
@@ -703,7 +703,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC1" authorId="0" shapeId="0" xr:uid="{3C8AC224-C308-41F9-9AF6-DC71515D8098}">
+    <comment ref="AE1" authorId="0" shapeId="0" xr:uid="{3C8AC224-C308-41F9-9AF6-DC71515D8098}">
       <text>
         <r>
           <rPr>
@@ -733,7 +733,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD1" authorId="0" shapeId="0" xr:uid="{5C0A6C82-6B8A-4ADD-AA15-F5F27C7C9B16}">
+    <comment ref="AF1" authorId="0" shapeId="0" xr:uid="{5C0A6C82-6B8A-4ADD-AA15-F5F27C7C9B16}">
       <text>
         <r>
           <rPr>
@@ -758,7 +758,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE1" authorId="0" shapeId="0" xr:uid="{795F82C3-4195-4E48-981C-501ABEED3CA8}">
+    <comment ref="AG1" authorId="0" shapeId="0" xr:uid="{795F82C3-4195-4E48-981C-501ABEED3CA8}">
       <text>
         <r>
           <rPr>
@@ -787,7 +787,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI1" authorId="0" shapeId="0" xr:uid="{B17F5182-5CD6-471A-802B-B04940EB1F07}">
+    <comment ref="AK1" authorId="0" shapeId="0" xr:uid="{B17F5182-5CD6-471A-802B-B04940EB1F07}">
       <text>
         <r>
           <rPr>
@@ -814,7 +814,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AJ1" authorId="0" shapeId="0" xr:uid="{83A64A19-0D57-4885-9A2C-DFE6B3D0CF3A}">
+    <comment ref="AL1" authorId="0" shapeId="0" xr:uid="{83A64A19-0D57-4885-9A2C-DFE6B3D0CF3A}">
       <text>
         <r>
           <rPr>
@@ -841,7 +841,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK1" authorId="0" shapeId="0" xr:uid="{C23793B6-57EA-4BE5-9374-0C67D52D0D5C}">
+    <comment ref="AM1" authorId="0" shapeId="0" xr:uid="{C23793B6-57EA-4BE5-9374-0C67D52D0D5C}">
       <text>
         <r>
           <rPr>
@@ -868,7 +868,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AL1" authorId="0" shapeId="0" xr:uid="{23EDBB42-EB78-4084-A22A-E2A320B7B718}">
+    <comment ref="AO1" authorId="0" shapeId="0" xr:uid="{23EDBB42-EB78-4084-A22A-E2A320B7B718}">
       <text>
         <r>
           <rPr>
@@ -894,7 +894,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM1" authorId="0" shapeId="0" xr:uid="{45483B7E-8619-46BA-A868-6DC1B5F0ED97}">
+    <comment ref="AP1" authorId="0" shapeId="0" xr:uid="{45483B7E-8619-46BA-A868-6DC1B5F0ED97}">
       <text>
         <r>
           <rPr>
@@ -920,7 +920,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN1" authorId="0" shapeId="0" xr:uid="{5BD000C3-A115-4E53-8A98-07117A910125}">
+    <comment ref="AQ1" authorId="0" shapeId="0" xr:uid="{5BD000C3-A115-4E53-8A98-07117A910125}">
       <text>
         <r>
           <rPr>
@@ -946,7 +946,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AO1" authorId="0" shapeId="0" xr:uid="{527DD670-6695-4116-85B3-1CE1EA2DA186}">
+    <comment ref="AR1" authorId="0" shapeId="0" xr:uid="{527DD670-6695-4116-85B3-1CE1EA2DA186}">
       <text>
         <r>
           <rPr>
@@ -972,7 +972,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP1" authorId="0" shapeId="0" xr:uid="{0CC13B28-9888-42DD-8F14-3A6BF2C85C1C}">
+    <comment ref="AS1" authorId="0" shapeId="0" xr:uid="{0CC13B28-9888-42DD-8F14-3A6BF2C85C1C}">
       <text>
         <r>
           <rPr>
@@ -998,7 +998,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AQ1" authorId="0" shapeId="0" xr:uid="{F075041D-AC35-4BDD-9FFC-350CC10834A2}">
+    <comment ref="AT1" authorId="0" shapeId="0" xr:uid="{F075041D-AC35-4BDD-9FFC-350CC10834A2}">
       <text>
         <r>
           <rPr>
@@ -1024,7 +1024,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AR1" authorId="0" shapeId="0" xr:uid="{333A9A2C-E124-41E6-9B23-490A99F08BC2}">
+    <comment ref="AU1" authorId="0" shapeId="0" xr:uid="{333A9A2C-E124-41E6-9B23-490A99F08BC2}">
       <text>
         <r>
           <rPr>
@@ -1050,7 +1050,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AS1" authorId="0" shapeId="0" xr:uid="{84379401-96F6-4E2F-BBE5-9AEA5930F1F7}">
+    <comment ref="AV1" authorId="0" shapeId="0" xr:uid="{84379401-96F6-4E2F-BBE5-9AEA5930F1F7}">
       <text>
         <r>
           <rPr>
@@ -1076,7 +1076,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AT1" authorId="0" shapeId="0" xr:uid="{F720710D-75B1-488B-81EF-656017BCBEC9}">
+    <comment ref="AW1" authorId="0" shapeId="0" xr:uid="{F720710D-75B1-488B-81EF-656017BCBEC9}">
       <text>
         <r>
           <rPr>
@@ -1102,7 +1102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU1" authorId="0" shapeId="0" xr:uid="{6B5BA4A9-A003-422D-BEA9-EB7231906A21}">
+    <comment ref="AX1" authorId="0" shapeId="0" xr:uid="{6B5BA4A9-A003-422D-BEA9-EB7231906A21}">
       <text>
         <r>
           <rPr>
@@ -1128,7 +1128,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AV1" authorId="0" shapeId="0" xr:uid="{A1695DDE-F786-4133-9E01-B711A4B3B5E0}">
+    <comment ref="AY1" authorId="0" shapeId="0" xr:uid="{A1695DDE-F786-4133-9E01-B711A4B3B5E0}">
       <text>
         <r>
           <rPr>
@@ -1154,7 +1154,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AX1" authorId="0" shapeId="0" xr:uid="{6E8A1D6E-E9E7-4730-96F4-42FCA2E3B89E}">
+    <comment ref="BA1" authorId="0" shapeId="0" xr:uid="{6E8A1D6E-E9E7-4730-96F4-42FCA2E3B89E}">
       <text>
         <r>
           <rPr>
@@ -1179,7 +1179,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AY1" authorId="0" shapeId="0" xr:uid="{B5624D4B-1D6E-41B2-B550-962F9614479A}">
+    <comment ref="BB1" authorId="0" shapeId="0" xr:uid="{B5624D4B-1D6E-41B2-B550-962F9614479A}">
       <text>
         <r>
           <rPr>
@@ -1204,7 +1204,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AZ1" authorId="0" shapeId="0" xr:uid="{8F72E90C-4BED-4038-997E-A10E8E8AA220}">
+    <comment ref="BC1" authorId="0" shapeId="0" xr:uid="{8F72E90C-4BED-4038-997E-A10E8E8AA220}">
       <text>
         <r>
           <rPr>
@@ -1229,7 +1229,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BA1" authorId="0" shapeId="0" xr:uid="{7D7262B2-604D-4B7F-8CCD-D4AD1EB59919}">
+    <comment ref="BD1" authorId="0" shapeId="0" xr:uid="{7D7262B2-604D-4B7F-8CCD-D4AD1EB59919}">
       <text>
         <r>
           <rPr>
@@ -1254,7 +1254,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BB1" authorId="0" shapeId="0" xr:uid="{8903C426-306A-4610-8322-B47368832A22}">
+    <comment ref="BE1" authorId="0" shapeId="0" xr:uid="{8903C426-306A-4610-8322-B47368832A22}">
       <text>
         <r>
           <rPr>
@@ -1279,7 +1279,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BC1" authorId="0" shapeId="0" xr:uid="{581ADCAD-C33E-4E29-A328-0CB4CAFA8386}">
+    <comment ref="BF1" authorId="0" shapeId="0" xr:uid="{581ADCAD-C33E-4E29-A328-0CB4CAFA8386}">
       <text>
         <r>
           <rPr>
@@ -1304,7 +1304,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BD1" authorId="0" shapeId="0" xr:uid="{2D74D483-8099-47E3-BB22-E0D0F1C8457F}">
+    <comment ref="BG1" authorId="0" shapeId="0" xr:uid="{2D74D483-8099-47E3-BB22-E0D0F1C8457F}">
       <text>
         <r>
           <rPr>
@@ -1334,7 +1334,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1226" uniqueCount="1156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="1159">
   <si>
     <t>Title</t>
   </si>
@@ -4802,6 +4802,15 @@
   </si>
   <si>
     <t>Islandora Document Content Model</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Table-Of-Contents</t>
+  </si>
+  <si>
+    <t>Subject-Local-Place</t>
   </si>
 </sst>
 </file>
@@ -5050,14 +5059,14 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5339,10 +5348,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BD1"/>
+  <dimension ref="A1:BG1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AE8" sqref="AE8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5354,30 +5363,30 @@
     <col min="5" max="5" width="21.140625" customWidth="1"/>
     <col min="6" max="6" width="42.42578125" customWidth="1"/>
     <col min="7" max="7" width="46.42578125" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" customWidth="1"/>
-    <col min="14" max="14" width="22" customWidth="1"/>
-    <col min="15" max="18" width="17.85546875" style="2" customWidth="1"/>
-    <col min="19" max="19" width="10.140625" customWidth="1"/>
-    <col min="20" max="21" width="14.42578125" customWidth="1"/>
-    <col min="22" max="23" width="11.140625" customWidth="1"/>
-    <col min="24" max="24" width="12.85546875" customWidth="1"/>
-    <col min="25" max="25" width="11.5703125" customWidth="1"/>
-    <col min="26" max="27" width="14.42578125" customWidth="1"/>
-    <col min="28" max="28" width="19.140625" customWidth="1"/>
-    <col min="29" max="29" width="18.5703125" customWidth="1"/>
-    <col min="30" max="30" width="12" customWidth="1"/>
-    <col min="35" max="35" width="16.140625" customWidth="1"/>
-    <col min="36" max="36" width="13.7109375" customWidth="1"/>
-    <col min="37" max="48" width="19.140625" customWidth="1"/>
-    <col min="49" max="49" width="25.7109375" customWidth="1"/>
-    <col min="50" max="53" width="23.28515625" customWidth="1"/>
-    <col min="55" max="55" width="16.28515625" customWidth="1"/>
-    <col min="56" max="56" width="13.140625" customWidth="1"/>
+    <col min="9" max="10" width="12.85546875" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" customWidth="1"/>
+    <col min="15" max="15" width="22" customWidth="1"/>
+    <col min="16" max="19" width="17.85546875" style="2" customWidth="1"/>
+    <col min="20" max="20" width="10.140625" customWidth="1"/>
+    <col min="21" max="22" width="14.42578125" customWidth="1"/>
+    <col min="23" max="24" width="11.140625" customWidth="1"/>
+    <col min="25" max="25" width="12.85546875" customWidth="1"/>
+    <col min="26" max="26" width="11.5703125" customWidth="1"/>
+    <col min="27" max="28" width="14.42578125" customWidth="1"/>
+    <col min="29" max="30" width="19.140625" customWidth="1"/>
+    <col min="31" max="31" width="18.5703125" customWidth="1"/>
+    <col min="32" max="32" width="12" customWidth="1"/>
+    <col min="37" max="37" width="16.140625" customWidth="1"/>
+    <col min="38" max="38" width="13.7109375" customWidth="1"/>
+    <col min="39" max="51" width="19.140625" customWidth="1"/>
+    <col min="52" max="52" width="25.7109375" customWidth="1"/>
+    <col min="53" max="56" width="23.28515625" customWidth="1"/>
+    <col min="58" max="58" width="16.28515625" customWidth="1"/>
+    <col min="59" max="59" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:59" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>16</v>
       </c>
@@ -5405,145 +5414,154 @@
       <c r="I1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="5" t="s">
+        <v>1156</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="AE1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AF1" s="9" t="s">
+      <c r="AH1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="AG1" s="9" t="s">
+      <c r="AI1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="AH1" s="9" t="s">
+      <c r="AJ1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="AL1" s="5" t="s">
+      <c r="AN1" s="3" t="s">
+        <v>1158</v>
+      </c>
+      <c r="AO1" s="5" t="s">
         <v>1138</v>
       </c>
-      <c r="AM1" s="5" t="s">
+      <c r="AP1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AN1" s="5" t="s">
+      <c r="AQ1" s="5" t="s">
         <v>1146</v>
       </c>
-      <c r="AO1" s="5" t="s">
+      <c r="AR1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AP1" s="5" t="s">
+      <c r="AS1" s="5" t="s">
         <v>1147</v>
       </c>
-      <c r="AQ1" s="5" t="s">
+      <c r="AT1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AR1" s="5" t="s">
+      <c r="AU1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="AS1" s="5" t="s">
+      <c r="AV1" s="5" t="s">
         <v>1148</v>
       </c>
-      <c r="AT1" s="5" t="s">
+      <c r="AW1" s="5" t="s">
         <v>1149</v>
       </c>
-      <c r="AU1" s="5" t="s">
+      <c r="AX1" s="5" t="s">
         <v>1150</v>
       </c>
-      <c r="AV1" s="5" t="s">
+      <c r="AY1" s="5" t="s">
         <v>1151</v>
       </c>
-      <c r="AW1" s="5" t="s">
+      <c r="AZ1" s="5" t="s">
         <v>1152</v>
       </c>
-      <c r="AX1" s="5" t="s">
+      <c r="BA1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="AY1" s="5" t="s">
+      <c r="BB1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AZ1" s="5" t="s">
+      <c r="BC1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="BA1" s="3" t="s">
+      <c r="BD1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="BB1" s="4" t="s">
+      <c r="BE1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="BC1" s="5" t="s">
+      <c r="BF1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="BD1" s="5" t="s">
+      <c r="BG1" s="5" t="s">
         <v>39</v>
       </c>
     </row>
@@ -5565,31 +5583,31 @@
           <x14:formula1>
             <xm:f>'Type list'!$A$1:$A$11</xm:f>
           </x14:formula1>
-          <xm:sqref>J2:J1048576</xm:sqref>
+          <xm:sqref>K2:K1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{220336D5-88C8-43FC-BAAF-0F62C8E76DFF}">
           <x14:formula1>
             <xm:f>'Date-Qualifier list'!$A$1:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>N2:N1048576</xm:sqref>
+          <xm:sqref>O2:O1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8D7091BA-978E-46FA-96E4-C1D3C047EB93}">
           <x14:formula1>
             <xm:f>'Digital-Origin list'!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>AA2:AA1048576</xm:sqref>
+          <xm:sqref>AB2:AB1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0775DFD4-8502-4F27-ACAE-32EBE7E704B0}">
           <x14:formula1>
             <xm:f>'Capture-Device list'!$A$1:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>AC2:AC1048576</xm:sqref>
+          <xm:sqref>AE2:AE1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D7E804B7-7CD0-4C17-8008-E4590082DA8A}">
           <x14:formula1>
             <xm:f>'Continent list'!$A$1:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>AL2:AL1048576</xm:sqref>
+          <xm:sqref>AO2:AO1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5612,7 +5630,7 @@
     <col min="3" max="3" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="69.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>48</v>
       </c>
@@ -5623,7 +5641,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="121.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>7</v>
       </c>
@@ -5634,7 +5652,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="121.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>53</v>
       </c>
@@ -5645,7 +5663,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="121.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>56</v>
       </c>
@@ -5656,7 +5674,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="104.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>59</v>
       </c>
@@ -5667,7 +5685,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="104.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>62</v>
       </c>
@@ -5678,7 +5696,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="104.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>65</v>
       </c>
@@ -5689,7 +5707,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="173.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>68</v>
       </c>
@@ -5700,7 +5718,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="104.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>68</v>
       </c>
@@ -5711,7 +5729,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="121.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>73</v>
       </c>
@@ -5722,7 +5740,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="138.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>73</v>
       </c>
@@ -5733,7 +5751,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="138.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>73</v>
       </c>
@@ -5744,7 +5762,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="138.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>80</v>
       </c>
@@ -5755,7 +5773,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="104.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>83</v>
       </c>
@@ -5766,7 +5784,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="104.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>83</v>
       </c>
@@ -5777,7 +5795,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="104.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>83</v>
       </c>
@@ -5788,7 +5806,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="121.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
         <v>83</v>
       </c>
@@ -5799,7 +5817,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="121.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>83</v>
       </c>
@@ -5822,13 +5840,13 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="18" t="s">
         <v>1154</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="18" t="s">
         <v>1155</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="18" t="s">
         <v>1153</v>
       </c>
     </row>
@@ -5990,7 +6008,7 @@
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="51" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>119</v>
       </c>
@@ -6006,7 +6024,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>123</v>
       </c>
@@ -6046,7 +6064,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="51" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>133</v>
       </c>
@@ -6098,7 +6116,7 @@
       <c r="A14" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="19" t="s">
         <v>147</v>
       </c>
     </row>
@@ -6106,7 +6124,7 @@
       <c r="A15" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="B15" s="19"/>
+      <c r="B15" s="20"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
@@ -6116,7 +6134,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="51" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>150</v>
       </c>
@@ -6140,7 +6158,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="51" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>156</v>
       </c>
@@ -6156,7 +6174,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>160</v>
       </c>
@@ -6172,7 +6190,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="102" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>164</v>
       </c>
@@ -6192,7 +6210,7 @@
       <c r="A26" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="19" t="s">
         <v>170</v>
       </c>
     </row>
@@ -6200,7 +6218,7 @@
       <c r="A27" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="B27" s="19"/>
+      <c r="B27" s="20"/>
     </row>
     <row r="28" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
@@ -6358,7 +6376,7 @@
       <c r="A47" s="15" t="s">
         <v>209</v>
       </c>
-      <c r="B47" s="18" t="s">
+      <c r="B47" s="19" t="s">
         <v>211</v>
       </c>
     </row>
@@ -6366,7 +6384,7 @@
       <c r="A48" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="B48" s="19"/>
+      <c r="B48" s="20"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
@@ -6484,7 +6502,7 @@
       <c r="A63" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B63" s="18" t="s">
+      <c r="B63" s="19" t="s">
         <v>242</v>
       </c>
     </row>
@@ -6492,7 +6510,7 @@
       <c r="A64" s="16" t="s">
         <v>241</v>
       </c>
-      <c r="B64" s="19"/>
+      <c r="B64" s="20"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
@@ -6554,7 +6572,7 @@
       <c r="A72" s="15" t="s">
         <v>257</v>
       </c>
-      <c r="B72" s="18" t="s">
+      <c r="B72" s="19" t="s">
         <v>259</v>
       </c>
     </row>
@@ -6562,7 +6580,7 @@
       <c r="A73" s="16" t="s">
         <v>258</v>
       </c>
-      <c r="B73" s="19"/>
+      <c r="B73" s="20"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="14" t="s">
@@ -6632,7 +6650,7 @@
       <c r="A82" s="15" t="s">
         <v>276</v>
       </c>
-      <c r="B82" s="18" t="s">
+      <c r="B82" s="19" t="s">
         <v>278</v>
       </c>
     </row>
@@ -6640,7 +6658,7 @@
       <c r="A83" s="16" t="s">
         <v>277</v>
       </c>
-      <c r="B83" s="19"/>
+      <c r="B83" s="20"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="14" t="s">
@@ -6678,7 +6696,7 @@
       <c r="A88" s="15" t="s">
         <v>287</v>
       </c>
-      <c r="B88" s="18" t="s">
+      <c r="B88" s="19" t="s">
         <v>289</v>
       </c>
     </row>
@@ -6686,7 +6704,7 @@
       <c r="A89" s="16" t="s">
         <v>288</v>
       </c>
-      <c r="B89" s="19"/>
+      <c r="B89" s="20"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="14" t="s">
@@ -6868,7 +6886,7 @@
       <c r="A112" s="15" t="s">
         <v>334</v>
       </c>
-      <c r="B112" s="18" t="s">
+      <c r="B112" s="19" t="s">
         <v>336</v>
       </c>
     </row>
@@ -6876,13 +6894,13 @@
       <c r="A113" s="16" t="s">
         <v>335</v>
       </c>
-      <c r="B113" s="19"/>
+      <c r="B113" s="20"/>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="15" t="s">
         <v>276</v>
       </c>
-      <c r="B114" s="18" t="s">
+      <c r="B114" s="19" t="s">
         <v>278</v>
       </c>
     </row>
@@ -6890,7 +6908,7 @@
       <c r="A115" s="16" t="s">
         <v>277</v>
       </c>
-      <c r="B115" s="19"/>
+      <c r="B115" s="20"/>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="14" t="s">
@@ -6944,7 +6962,7 @@
       <c r="A122" s="15" t="s">
         <v>349</v>
       </c>
-      <c r="B122" s="18" t="s">
+      <c r="B122" s="19" t="s">
         <v>351</v>
       </c>
     </row>
@@ -6952,7 +6970,7 @@
       <c r="A123" s="16" t="s">
         <v>350</v>
       </c>
-      <c r="B123" s="19"/>
+      <c r="B123" s="20"/>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="14" t="s">
@@ -7022,7 +7040,7 @@
       <c r="A132" s="15" t="s">
         <v>368</v>
       </c>
-      <c r="B132" s="18" t="s">
+      <c r="B132" s="19" t="s">
         <v>370</v>
       </c>
     </row>
@@ -7030,7 +7048,7 @@
       <c r="A133" s="16" t="s">
         <v>369</v>
       </c>
-      <c r="B133" s="19"/>
+      <c r="B133" s="20"/>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="14" t="s">
@@ -7076,7 +7094,7 @@
       <c r="A139" s="15" t="s">
         <v>381</v>
       </c>
-      <c r="B139" s="18" t="s">
+      <c r="B139" s="19" t="s">
         <v>383</v>
       </c>
     </row>
@@ -7084,7 +7102,7 @@
       <c r="A140" s="16" t="s">
         <v>382</v>
       </c>
-      <c r="B140" s="19"/>
+      <c r="B140" s="20"/>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="14" t="s">
@@ -7130,7 +7148,7 @@
       <c r="A146" s="15" t="s">
         <v>209</v>
       </c>
-      <c r="B146" s="18" t="s">
+      <c r="B146" s="19" t="s">
         <v>211</v>
       </c>
     </row>
@@ -7138,7 +7156,7 @@
       <c r="A147" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="B147" s="19"/>
+      <c r="B147" s="20"/>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="14" t="s">
@@ -7176,7 +7194,7 @@
       <c r="A152" s="15" t="s">
         <v>402</v>
       </c>
-      <c r="B152" s="18" t="s">
+      <c r="B152" s="19" t="s">
         <v>404</v>
       </c>
     </row>
@@ -7184,7 +7202,7 @@
       <c r="A153" s="16" t="s">
         <v>403</v>
       </c>
-      <c r="B153" s="19"/>
+      <c r="B153" s="20"/>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="14" t="s">
@@ -7238,7 +7256,7 @@
       <c r="A160" s="15" t="s">
         <v>417</v>
       </c>
-      <c r="B160" s="18" t="s">
+      <c r="B160" s="19" t="s">
         <v>419</v>
       </c>
     </row>
@@ -7246,13 +7264,13 @@
       <c r="A161" s="16" t="s">
         <v>418</v>
       </c>
-      <c r="B161" s="19"/>
+      <c r="B161" s="20"/>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="15" t="s">
         <v>417</v>
       </c>
-      <c r="B162" s="18" t="s">
+      <c r="B162" s="19" t="s">
         <v>419</v>
       </c>
     </row>
@@ -7260,7 +7278,7 @@
       <c r="A163" s="16" t="s">
         <v>418</v>
       </c>
-      <c r="B163" s="19"/>
+      <c r="B163" s="20"/>
     </row>
     <row r="164" spans="1:2" ht="51" x14ac:dyDescent="0.25">
       <c r="A164" s="14" t="s">
@@ -7354,7 +7372,7 @@
       <c r="A175" s="15" t="s">
         <v>442</v>
       </c>
-      <c r="B175" s="18" t="s">
+      <c r="B175" s="19" t="s">
         <v>444</v>
       </c>
     </row>
@@ -7362,13 +7380,13 @@
       <c r="A176" s="16" t="s">
         <v>443</v>
       </c>
-      <c r="B176" s="19"/>
+      <c r="B176" s="20"/>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="15" t="s">
         <v>349</v>
       </c>
-      <c r="B177" s="18" t="s">
+      <c r="B177" s="19" t="s">
         <v>351</v>
       </c>
     </row>
@@ -7376,7 +7394,7 @@
       <c r="A178" s="16" t="s">
         <v>350</v>
       </c>
-      <c r="B178" s="19"/>
+      <c r="B178" s="20"/>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="14" t="s">
@@ -7486,7 +7504,7 @@
       <c r="A192" s="15" t="s">
         <v>381</v>
       </c>
-      <c r="B192" s="18" t="s">
+      <c r="B192" s="19" t="s">
         <v>383</v>
       </c>
     </row>
@@ -7494,7 +7512,7 @@
       <c r="A193" s="16" t="s">
         <v>382</v>
       </c>
-      <c r="B193" s="19"/>
+      <c r="B193" s="20"/>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="14" t="s">
@@ -7660,7 +7678,7 @@
       <c r="A214" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="B214" s="18" t="s">
+      <c r="B214" s="19" t="s">
         <v>170</v>
       </c>
     </row>
@@ -7668,7 +7686,7 @@
       <c r="A215" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="B215" s="19"/>
+      <c r="B215" s="20"/>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" s="14" t="s">
@@ -7690,7 +7708,7 @@
       <c r="A218" s="15" t="s">
         <v>515</v>
       </c>
-      <c r="B218" s="18" t="s">
+      <c r="B218" s="19" t="s">
         <v>517</v>
       </c>
     </row>
@@ -7698,7 +7716,7 @@
       <c r="A219" s="16" t="s">
         <v>516</v>
       </c>
-      <c r="B219" s="19"/>
+      <c r="B219" s="20"/>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" s="14" t="s">
@@ -7816,7 +7834,7 @@
       <c r="A234" s="15" t="s">
         <v>515</v>
       </c>
-      <c r="B234" s="18" t="s">
+      <c r="B234" s="19" t="s">
         <v>517</v>
       </c>
     </row>
@@ -7824,7 +7842,7 @@
       <c r="A235" s="16" t="s">
         <v>516</v>
       </c>
-      <c r="B235" s="19"/>
+      <c r="B235" s="20"/>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" s="14" t="s">
@@ -7942,7 +7960,7 @@
       <c r="A250" s="15" t="s">
         <v>442</v>
       </c>
-      <c r="B250" s="18" t="s">
+      <c r="B250" s="19" t="s">
         <v>444</v>
       </c>
     </row>
@@ -7950,7 +7968,7 @@
       <c r="A251" s="16" t="s">
         <v>443</v>
       </c>
-      <c r="B251" s="19"/>
+      <c r="B251" s="20"/>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" s="14" t="s">
@@ -8324,7 +8342,7 @@
       <c r="A298" s="15" t="s">
         <v>666</v>
       </c>
-      <c r="B298" s="18" t="s">
+      <c r="B298" s="19" t="s">
         <v>668</v>
       </c>
     </row>
@@ -8332,7 +8350,7 @@
       <c r="A299" s="16" t="s">
         <v>667</v>
       </c>
-      <c r="B299" s="19"/>
+      <c r="B299" s="20"/>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A300" s="14" t="s">
@@ -8394,7 +8412,7 @@
       <c r="A307" s="15" t="s">
         <v>683</v>
       </c>
-      <c r="B307" s="18" t="s">
+      <c r="B307" s="19" t="s">
         <v>685</v>
       </c>
     </row>
@@ -8402,7 +8420,7 @@
       <c r="A308" s="16" t="s">
         <v>684</v>
       </c>
-      <c r="B308" s="19"/>
+      <c r="B308" s="20"/>
     </row>
     <row r="309" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A309" s="14" t="s">
@@ -8432,7 +8450,7 @@
       <c r="A312" s="15" t="s">
         <v>692</v>
       </c>
-      <c r="B312" s="18" t="s">
+      <c r="B312" s="19" t="s">
         <v>694</v>
       </c>
     </row>
@@ -8440,7 +8458,7 @@
       <c r="A313" s="16" t="s">
         <v>693</v>
       </c>
-      <c r="B313" s="19"/>
+      <c r="B313" s="20"/>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A314" s="14" t="s">
@@ -8502,7 +8520,7 @@
       <c r="A321" s="15" t="s">
         <v>666</v>
       </c>
-      <c r="B321" s="18" t="s">
+      <c r="B321" s="19" t="s">
         <v>668</v>
       </c>
     </row>
@@ -8510,7 +8528,7 @@
       <c r="A322" s="16" t="s">
         <v>667</v>
       </c>
-      <c r="B322" s="19"/>
+      <c r="B322" s="20"/>
     </row>
     <row r="323" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A323" s="14" t="s">
@@ -8588,7 +8606,7 @@
       <c r="A332" s="15" t="s">
         <v>683</v>
       </c>
-      <c r="B332" s="18" t="s">
+      <c r="B332" s="19" t="s">
         <v>685</v>
       </c>
     </row>
@@ -8596,13 +8614,13 @@
       <c r="A333" s="16" t="s">
         <v>684</v>
       </c>
-      <c r="B333" s="19"/>
+      <c r="B333" s="20"/>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A334" s="15" t="s">
         <v>692</v>
       </c>
-      <c r="B334" s="18" t="s">
+      <c r="B334" s="19" t="s">
         <v>694</v>
       </c>
     </row>
@@ -8610,7 +8628,7 @@
       <c r="A335" s="16" t="s">
         <v>693</v>
       </c>
-      <c r="B335" s="19"/>
+      <c r="B335" s="20"/>
     </row>
     <row r="336" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A336" s="14" t="s">
@@ -8656,7 +8674,7 @@
       <c r="A341" s="15" t="s">
         <v>257</v>
       </c>
-      <c r="B341" s="18" t="s">
+      <c r="B341" s="19" t="s">
         <v>259</v>
       </c>
     </row>
@@ -8664,7 +8682,7 @@
       <c r="A342" s="16" t="s">
         <v>258</v>
       </c>
-      <c r="B342" s="19"/>
+      <c r="B342" s="20"/>
     </row>
     <row r="343" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A343" s="14" t="s">
@@ -8798,7 +8816,7 @@
       <c r="A359" s="15" t="s">
         <v>368</v>
       </c>
-      <c r="B359" s="18" t="s">
+      <c r="B359" s="19" t="s">
         <v>370</v>
       </c>
     </row>
@@ -8806,7 +8824,7 @@
       <c r="A360" s="16" t="s">
         <v>369</v>
       </c>
-      <c r="B360" s="19"/>
+      <c r="B360" s="20"/>
     </row>
     <row r="361" spans="1:2" ht="51" x14ac:dyDescent="0.25">
       <c r="A361" s="14" t="s">
@@ -9052,7 +9070,7 @@
       <c r="A391" s="15" t="s">
         <v>402</v>
       </c>
-      <c r="B391" s="18" t="s">
+      <c r="B391" s="19" t="s">
         <v>404</v>
       </c>
     </row>
@@ -9060,7 +9078,7 @@
       <c r="A392" s="16" t="s">
         <v>403</v>
       </c>
-      <c r="B392" s="19"/>
+      <c r="B392" s="20"/>
     </row>
     <row r="393" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A393" s="14" t="s">
@@ -9202,7 +9220,7 @@
       <c r="A410" s="15" t="s">
         <v>863</v>
       </c>
-      <c r="B410" s="18" t="s">
+      <c r="B410" s="19" t="s">
         <v>865</v>
       </c>
     </row>
@@ -9210,13 +9228,13 @@
       <c r="A411" s="16" t="s">
         <v>864</v>
       </c>
-      <c r="B411" s="19"/>
+      <c r="B411" s="20"/>
     </row>
     <row r="412" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A412" s="15" t="s">
         <v>863</v>
       </c>
-      <c r="B412" s="18" t="s">
+      <c r="B412" s="19" t="s">
         <v>865</v>
       </c>
     </row>
@@ -9224,7 +9242,7 @@
       <c r="A413" s="16" t="s">
         <v>864</v>
       </c>
-      <c r="B413" s="19"/>
+      <c r="B413" s="20"/>
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A414" s="14" t="s">
@@ -9422,7 +9440,7 @@
       <c r="A438" s="15" t="s">
         <v>914</v>
       </c>
-      <c r="B438" s="18" t="s">
+      <c r="B438" s="19" t="s">
         <v>916</v>
       </c>
     </row>
@@ -9430,13 +9448,13 @@
       <c r="A439" s="16" t="s">
         <v>915</v>
       </c>
-      <c r="B439" s="19"/>
+      <c r="B439" s="20"/>
     </row>
     <row r="440" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A440" s="15" t="s">
         <v>914</v>
       </c>
-      <c r="B440" s="18" t="s">
+      <c r="B440" s="19" t="s">
         <v>916</v>
       </c>
     </row>
@@ -9444,7 +9462,7 @@
       <c r="A441" s="16" t="s">
         <v>915</v>
       </c>
-      <c r="B441" s="19"/>
+      <c r="B441" s="20"/>
     </row>
     <row r="442" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A442" s="14" t="s">
@@ -9578,7 +9596,7 @@
       <c r="A458" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="B458" s="18" t="s">
+      <c r="B458" s="19" t="s">
         <v>147</v>
       </c>
     </row>
@@ -9586,7 +9604,7 @@
       <c r="A459" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="B459" s="19"/>
+      <c r="B459" s="20"/>
     </row>
     <row r="460" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A460" s="14" t="s">
@@ -9792,7 +9810,7 @@
       <c r="A485" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B485" s="18" t="s">
+      <c r="B485" s="19" t="s">
         <v>242</v>
       </c>
     </row>
@@ -9800,7 +9818,7 @@
       <c r="A486" s="16" t="s">
         <v>241</v>
       </c>
-      <c r="B486" s="19"/>
+      <c r="B486" s="20"/>
     </row>
     <row r="487" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A487" s="14" t="s">
@@ -10110,7 +10128,7 @@
       <c r="A525" s="15" t="s">
         <v>334</v>
       </c>
-      <c r="B525" s="18" t="s">
+      <c r="B525" s="19" t="s">
         <v>336</v>
       </c>
     </row>
@@ -10118,7 +10136,7 @@
       <c r="A526" s="16" t="s">
         <v>335</v>
       </c>
-      <c r="B526" s="19"/>
+      <c r="B526" s="20"/>
     </row>
     <row r="527" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A527" s="14" t="s">
@@ -10244,7 +10262,7 @@
       <c r="A542" s="15" t="s">
         <v>287</v>
       </c>
-      <c r="B542" s="18" t="s">
+      <c r="B542" s="19" t="s">
         <v>289</v>
       </c>
     </row>
@@ -10252,7 +10270,7 @@
       <c r="A543" s="16" t="s">
         <v>288</v>
       </c>
-      <c r="B543" s="19"/>
+      <c r="B543" s="20"/>
     </row>
     <row r="544" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A544" s="14" t="s">

</xml_diff>

<commit_message>
Added label and photo fields
</commit_message>
<xml_diff>
--- a/digitalcollections-standard-metadata.xlsx
+++ b/digitalcollections-standard-metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Lehigh\Work From Home\Spreadsheet\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Work\Work From Home\Spreadsheet\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70EBA08A-DB02-4ECD-8EAB-8AF7757ED315}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F526C6D-1B8C-498F-B169-3FDE71B1A9FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="60" windowWidth="28800" windowHeight="15210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Islandora Metadata Template" sheetId="1" r:id="rId1"/>
@@ -142,7 +142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{28CCD625-11F1-4A9A-9F99-86D753960E41}">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{28CCD625-11F1-4A9A-9F99-86D753960E41}">
       <text>
         <r>
           <rPr>
@@ -166,7 +166,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{64D5C3CE-3911-4086-B0DF-90859684B90F}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{64D5C3CE-3911-4086-B0DF-90859684B90F}">
       <text>
         <r>
           <rPr>
@@ -192,7 +192,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{1C97156B-ECD1-4A9F-A796-AA0F9A759A74}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{1C97156B-ECD1-4A9F-A796-AA0F9A759A74}">
       <text>
         <r>
           <rPr>
@@ -216,7 +216,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{A45955F0-C447-4E97-A7BA-BD50D6CFDEEA}">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{A45955F0-C447-4E97-A7BA-BD50D6CFDEEA}">
       <text>
         <r>
           <rPr>
@@ -242,7 +242,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{454DE92F-D709-4465-BBD9-0A87F9FE3884}">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{454DE92F-D709-4465-BBD9-0A87F9FE3884}">
       <text>
         <r>
           <rPr>
@@ -268,7 +268,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{B54B678A-3085-4E00-B156-EEE7F291535C}">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{B54B678A-3085-4E00-B156-EEE7F291535C}">
       <text>
         <r>
           <rPr>
@@ -293,7 +293,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{63A938D5-DD9F-4C28-85B7-862F01C2557B}">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{63A938D5-DD9F-4C28-85B7-862F01C2557B}">
       <text>
         <r>
           <rPr>
@@ -319,7 +319,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{F3FC3F32-7AD5-4AD5-BC96-E284BC31D639}">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{F3FC3F32-7AD5-4AD5-BC96-E284BC31D639}">
       <text>
         <r>
           <rPr>
@@ -346,7 +346,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{C8C7F5BA-7F77-486D-89C1-EE8841EBF865}">
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{C8C7F5BA-7F77-486D-89C1-EE8841EBF865}">
       <text>
         <r>
           <rPr>
@@ -372,7 +372,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{E3B509DE-43E9-44B5-BDEC-98F9565127F8}">
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{E3B509DE-43E9-44B5-BDEC-98F9565127F8}">
       <text>
         <r>
           <rPr>
@@ -396,7 +396,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{E2CC8CA8-D47F-4EEC-A37F-5713BAB9E324}">
+    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{E2CC8CA8-D47F-4EEC-A37F-5713BAB9E324}">
       <text>
         <r>
           <rPr>
@@ -420,7 +420,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{091FF495-4462-4CC1-8F23-39AEEA05BB0A}">
+    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{091FF495-4462-4CC1-8F23-39AEEA05BB0A}">
       <text>
         <r>
           <rPr>
@@ -446,7 +446,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{E08F8DEB-76A8-4E0E-966F-F84105839B5D}">
+    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{E08F8DEB-76A8-4E0E-966F-F84105839B5D}">
       <text>
         <r>
           <rPr>
@@ -470,7 +470,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{C37A58A6-F5F3-40F1-A828-7C18B781422F}">
+    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{C37A58A6-F5F3-40F1-A828-7C18B781422F}">
       <text>
         <r>
           <rPr>
@@ -496,7 +496,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{3991E12B-3A71-4A97-B3B5-1180C0193E47}">
+    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{3991E12B-3A71-4A97-B3B5-1180C0193E47}">
       <text>
         <r>
           <rPr>
@@ -522,7 +522,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{85E6D484-5A90-45DD-9A06-ACAEA4E36301}">
+    <comment ref="X1" authorId="0" shapeId="0" xr:uid="{85E6D484-5A90-45DD-9A06-ACAEA4E36301}">
       <text>
         <r>
           <rPr>
@@ -548,7 +548,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0" shapeId="0" xr:uid="{F6F51BBE-97C7-4474-9B6A-5F28B5E6742F}">
+    <comment ref="Y1" authorId="0" shapeId="0" xr:uid="{F6F51BBE-97C7-4474-9B6A-5F28B5E6742F}">
       <text>
         <r>
           <rPr>
@@ -573,7 +573,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="0" shapeId="0" xr:uid="{4BBD92AC-9B74-421C-B77E-49175DBE1818}">
+    <comment ref="Z1" authorId="0" shapeId="0" xr:uid="{4BBD92AC-9B74-421C-B77E-49175DBE1818}">
       <text>
         <r>
           <rPr>
@@ -599,7 +599,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="0" shapeId="0" xr:uid="{A13F7FB5-2D79-4361-A957-990F73831417}">
+    <comment ref="AA1" authorId="0" shapeId="0" xr:uid="{A13F7FB5-2D79-4361-A957-990F73831417}">
       <text>
         <r>
           <rPr>
@@ -624,7 +624,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA1" authorId="0" shapeId="0" xr:uid="{6FFEBC39-3422-4FA0-98D2-223893A185AA}">
+    <comment ref="AB1" authorId="0" shapeId="0" xr:uid="{6FFEBC39-3422-4FA0-98D2-223893A185AA}">
       <text>
         <r>
           <rPr>
@@ -650,7 +650,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB1" authorId="0" shapeId="0" xr:uid="{5D40D71D-7BB4-4B93-99E1-B2FD752A62E9}">
+    <comment ref="AC1" authorId="0" shapeId="0" xr:uid="{5D40D71D-7BB4-4B93-99E1-B2FD752A62E9}">
       <text>
         <r>
           <rPr>
@@ -679,7 +679,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC1" authorId="0" shapeId="0" xr:uid="{FC850D2C-B335-4894-B732-C94221F61B96}">
+    <comment ref="AD1" authorId="0" shapeId="0" xr:uid="{FC850D2C-B335-4894-B732-C94221F61B96}">
       <text>
         <r>
           <rPr>
@@ -703,7 +703,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE1" authorId="0" shapeId="0" xr:uid="{3C8AC224-C308-41F9-9AF6-DC71515D8098}">
+    <comment ref="AF1" authorId="0" shapeId="0" xr:uid="{3C8AC224-C308-41F9-9AF6-DC71515D8098}">
       <text>
         <r>
           <rPr>
@@ -733,7 +733,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF1" authorId="0" shapeId="0" xr:uid="{5C0A6C82-6B8A-4ADD-AA15-F5F27C7C9B16}">
+    <comment ref="AG1" authorId="0" shapeId="0" xr:uid="{5C0A6C82-6B8A-4ADD-AA15-F5F27C7C9B16}">
       <text>
         <r>
           <rPr>
@@ -758,7 +758,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG1" authorId="0" shapeId="0" xr:uid="{795F82C3-4195-4E48-981C-501ABEED3CA8}">
+    <comment ref="AH1" authorId="0" shapeId="0" xr:uid="{795F82C3-4195-4E48-981C-501ABEED3CA8}">
       <text>
         <r>
           <rPr>
@@ -787,7 +787,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK1" authorId="0" shapeId="0" xr:uid="{B17F5182-5CD6-471A-802B-B04940EB1F07}">
+    <comment ref="AL1" authorId="0" shapeId="0" xr:uid="{B17F5182-5CD6-471A-802B-B04940EB1F07}">
       <text>
         <r>
           <rPr>
@@ -814,7 +814,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AL1" authorId="0" shapeId="0" xr:uid="{83A64A19-0D57-4885-9A2C-DFE6B3D0CF3A}">
+    <comment ref="AM1" authorId="0" shapeId="0" xr:uid="{83A64A19-0D57-4885-9A2C-DFE6B3D0CF3A}">
       <text>
         <r>
           <rPr>
@@ -841,7 +841,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM1" authorId="0" shapeId="0" xr:uid="{C23793B6-57EA-4BE5-9374-0C67D52D0D5C}">
+    <comment ref="AN1" authorId="0" shapeId="0" xr:uid="{C23793B6-57EA-4BE5-9374-0C67D52D0D5C}">
       <text>
         <r>
           <rPr>
@@ -868,7 +868,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AO1" authorId="0" shapeId="0" xr:uid="{23EDBB42-EB78-4084-A22A-E2A320B7B718}">
+    <comment ref="AP1" authorId="0" shapeId="0" xr:uid="{23EDBB42-EB78-4084-A22A-E2A320B7B718}">
       <text>
         <r>
           <rPr>
@@ -894,7 +894,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP1" authorId="0" shapeId="0" xr:uid="{45483B7E-8619-46BA-A868-6DC1B5F0ED97}">
+    <comment ref="AQ1" authorId="0" shapeId="0" xr:uid="{45483B7E-8619-46BA-A868-6DC1B5F0ED97}">
       <text>
         <r>
           <rPr>
@@ -920,7 +920,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AQ1" authorId="0" shapeId="0" xr:uid="{5BD000C3-A115-4E53-8A98-07117A910125}">
+    <comment ref="AR1" authorId="0" shapeId="0" xr:uid="{5BD000C3-A115-4E53-8A98-07117A910125}">
       <text>
         <r>
           <rPr>
@@ -946,7 +946,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AR1" authorId="0" shapeId="0" xr:uid="{527DD670-6695-4116-85B3-1CE1EA2DA186}">
+    <comment ref="AS1" authorId="0" shapeId="0" xr:uid="{527DD670-6695-4116-85B3-1CE1EA2DA186}">
       <text>
         <r>
           <rPr>
@@ -972,7 +972,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AS1" authorId="0" shapeId="0" xr:uid="{0CC13B28-9888-42DD-8F14-3A6BF2C85C1C}">
+    <comment ref="AT1" authorId="0" shapeId="0" xr:uid="{0CC13B28-9888-42DD-8F14-3A6BF2C85C1C}">
       <text>
         <r>
           <rPr>
@@ -998,7 +998,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AT1" authorId="0" shapeId="0" xr:uid="{F075041D-AC35-4BDD-9FFC-350CC10834A2}">
+    <comment ref="AU1" authorId="0" shapeId="0" xr:uid="{F075041D-AC35-4BDD-9FFC-350CC10834A2}">
       <text>
         <r>
           <rPr>
@@ -1024,7 +1024,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU1" authorId="0" shapeId="0" xr:uid="{333A9A2C-E124-41E6-9B23-490A99F08BC2}">
+    <comment ref="AV1" authorId="0" shapeId="0" xr:uid="{333A9A2C-E124-41E6-9B23-490A99F08BC2}">
       <text>
         <r>
           <rPr>
@@ -1050,7 +1050,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AV1" authorId="0" shapeId="0" xr:uid="{84379401-96F6-4E2F-BBE5-9AEA5930F1F7}">
+    <comment ref="AW1" authorId="0" shapeId="0" xr:uid="{84379401-96F6-4E2F-BBE5-9AEA5930F1F7}">
       <text>
         <r>
           <rPr>
@@ -1076,7 +1076,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AW1" authorId="0" shapeId="0" xr:uid="{F720710D-75B1-488B-81EF-656017BCBEC9}">
+    <comment ref="AX1" authorId="0" shapeId="0" xr:uid="{F720710D-75B1-488B-81EF-656017BCBEC9}">
       <text>
         <r>
           <rPr>
@@ -1102,7 +1102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AX1" authorId="0" shapeId="0" xr:uid="{6B5BA4A9-A003-422D-BEA9-EB7231906A21}">
+    <comment ref="AY1" authorId="0" shapeId="0" xr:uid="{6B5BA4A9-A003-422D-BEA9-EB7231906A21}">
       <text>
         <r>
           <rPr>
@@ -1128,7 +1128,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AY1" authorId="0" shapeId="0" xr:uid="{A1695DDE-F786-4133-9E01-B711A4B3B5E0}">
+    <comment ref="AZ1" authorId="0" shapeId="0" xr:uid="{A1695DDE-F786-4133-9E01-B711A4B3B5E0}">
       <text>
         <r>
           <rPr>
@@ -1154,7 +1154,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BA1" authorId="0" shapeId="0" xr:uid="{6E8A1D6E-E9E7-4730-96F4-42FCA2E3B89E}">
+    <comment ref="BB1" authorId="0" shapeId="0" xr:uid="{6E8A1D6E-E9E7-4730-96F4-42FCA2E3B89E}">
       <text>
         <r>
           <rPr>
@@ -1179,7 +1179,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BB1" authorId="0" shapeId="0" xr:uid="{B5624D4B-1D6E-41B2-B550-962F9614479A}">
+    <comment ref="BC1" authorId="0" shapeId="0" xr:uid="{B5624D4B-1D6E-41B2-B550-962F9614479A}">
       <text>
         <r>
           <rPr>
@@ -1204,7 +1204,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BC1" authorId="0" shapeId="0" xr:uid="{8F72E90C-4BED-4038-997E-A10E8E8AA220}">
+    <comment ref="BD1" authorId="0" shapeId="0" xr:uid="{8F72E90C-4BED-4038-997E-A10E8E8AA220}">
       <text>
         <r>
           <rPr>
@@ -1229,7 +1229,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BD1" authorId="0" shapeId="0" xr:uid="{7D7262B2-604D-4B7F-8CCD-D4AD1EB59919}">
+    <comment ref="BE1" authorId="0" shapeId="0" xr:uid="{7D7262B2-604D-4B7F-8CCD-D4AD1EB59919}">
       <text>
         <r>
           <rPr>
@@ -1254,7 +1254,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BE1" authorId="0" shapeId="0" xr:uid="{8903C426-306A-4610-8322-B47368832A22}">
+    <comment ref="BF1" authorId="0" shapeId="0" xr:uid="{8903C426-306A-4610-8322-B47368832A22}">
       <text>
         <r>
           <rPr>
@@ -1279,7 +1279,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BF1" authorId="0" shapeId="0" xr:uid="{581ADCAD-C33E-4E29-A328-0CB4CAFA8386}">
+    <comment ref="BG1" authorId="0" shapeId="0" xr:uid="{581ADCAD-C33E-4E29-A328-0CB4CAFA8386}">
       <text>
         <r>
           <rPr>
@@ -1304,7 +1304,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BG1" authorId="0" shapeId="0" xr:uid="{2D74D483-8099-47E3-BB22-E0D0F1C8457F}">
+    <comment ref="BH1" authorId="0" shapeId="0" xr:uid="{2D74D483-8099-47E3-BB22-E0D0F1C8457F}">
       <text>
         <r>
           <rPr>
@@ -1334,7 +1334,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="1159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1230" uniqueCount="1160">
   <si>
     <t>Title</t>
   </si>
@@ -4811,6 +4811,9 @@
   </si>
   <si>
     <t>Subject-Local-Place</t>
+  </si>
+  <si>
+    <t>label</t>
   </si>
 </sst>
 </file>
@@ -5348,10 +5351,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BG1"/>
+  <dimension ref="A1:BH1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AE8" sqref="AE8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5361,32 +5364,32 @@
     <col min="3" max="3" width="9.5703125" customWidth="1"/>
     <col min="4" max="4" width="34.28515625" customWidth="1"/>
     <col min="5" max="5" width="21.140625" customWidth="1"/>
-    <col min="6" max="6" width="42.42578125" customWidth="1"/>
-    <col min="7" max="7" width="46.42578125" customWidth="1"/>
-    <col min="9" max="10" width="12.85546875" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" customWidth="1"/>
-    <col min="15" max="15" width="22" customWidth="1"/>
-    <col min="16" max="19" width="17.85546875" style="2" customWidth="1"/>
-    <col min="20" max="20" width="10.140625" customWidth="1"/>
-    <col min="21" max="22" width="14.42578125" customWidth="1"/>
-    <col min="23" max="24" width="11.140625" customWidth="1"/>
-    <col min="25" max="25" width="12.85546875" customWidth="1"/>
-    <col min="26" max="26" width="11.5703125" customWidth="1"/>
-    <col min="27" max="28" width="14.42578125" customWidth="1"/>
-    <col min="29" max="30" width="19.140625" customWidth="1"/>
-    <col min="31" max="31" width="18.5703125" customWidth="1"/>
-    <col min="32" max="32" width="12" customWidth="1"/>
-    <col min="37" max="37" width="16.140625" customWidth="1"/>
-    <col min="38" max="38" width="13.7109375" customWidth="1"/>
-    <col min="39" max="51" width="19.140625" customWidth="1"/>
-    <col min="52" max="52" width="25.7109375" customWidth="1"/>
-    <col min="53" max="56" width="23.28515625" customWidth="1"/>
-    <col min="58" max="58" width="16.28515625" customWidth="1"/>
-    <col min="59" max="59" width="13.140625" customWidth="1"/>
+    <col min="6" max="7" width="42.42578125" customWidth="1"/>
+    <col min="8" max="8" width="46.42578125" customWidth="1"/>
+    <col min="10" max="11" width="12.85546875" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" customWidth="1"/>
+    <col min="16" max="16" width="22" customWidth="1"/>
+    <col min="17" max="20" width="17.85546875" style="2" customWidth="1"/>
+    <col min="21" max="21" width="10.140625" customWidth="1"/>
+    <col min="22" max="23" width="14.42578125" customWidth="1"/>
+    <col min="24" max="25" width="11.140625" customWidth="1"/>
+    <col min="26" max="26" width="12.85546875" customWidth="1"/>
+    <col min="27" max="27" width="11.5703125" customWidth="1"/>
+    <col min="28" max="29" width="14.42578125" customWidth="1"/>
+    <col min="30" max="31" width="19.140625" customWidth="1"/>
+    <col min="32" max="32" width="18.5703125" customWidth="1"/>
+    <col min="33" max="33" width="12" customWidth="1"/>
+    <col min="38" max="38" width="16.140625" customWidth="1"/>
+    <col min="39" max="39" width="13.7109375" customWidth="1"/>
+    <col min="40" max="52" width="19.140625" customWidth="1"/>
+    <col min="53" max="53" width="25.7109375" customWidth="1"/>
+    <col min="54" max="57" width="23.28515625" customWidth="1"/>
+    <col min="59" max="59" width="16.28515625" customWidth="1"/>
+    <col min="60" max="60" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:60" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>16</v>
       </c>
@@ -5406,162 +5409,165 @@
         <v>21</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>1159</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>1156</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="S1" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="T1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>1157</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AH1" s="9" t="s">
+      <c r="AI1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="AI1" s="9" t="s">
+      <c r="AJ1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="AJ1" s="9" t="s">
+      <c r="AK1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>1158</v>
       </c>
-      <c r="AO1" s="5" t="s">
+      <c r="AP1" s="5" t="s">
         <v>1138</v>
       </c>
-      <c r="AP1" s="5" t="s">
+      <c r="AQ1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AQ1" s="5" t="s">
+      <c r="AR1" s="5" t="s">
         <v>1146</v>
       </c>
-      <c r="AR1" s="5" t="s">
+      <c r="AS1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AS1" s="5" t="s">
+      <c r="AT1" s="5" t="s">
         <v>1147</v>
       </c>
-      <c r="AT1" s="5" t="s">
+      <c r="AU1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AU1" s="5" t="s">
+      <c r="AV1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="AV1" s="5" t="s">
+      <c r="AW1" s="5" t="s">
         <v>1148</v>
       </c>
-      <c r="AW1" s="5" t="s">
+      <c r="AX1" s="5" t="s">
         <v>1149</v>
       </c>
-      <c r="AX1" s="5" t="s">
+      <c r="AY1" s="5" t="s">
         <v>1150</v>
       </c>
-      <c r="AY1" s="5" t="s">
+      <c r="AZ1" s="5" t="s">
         <v>1151</v>
       </c>
-      <c r="AZ1" s="5" t="s">
+      <c r="BA1" s="5" t="s">
         <v>1152</v>
       </c>
-      <c r="BA1" s="5" t="s">
+      <c r="BB1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="BB1" s="5" t="s">
+      <c r="BC1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="BC1" s="5" t="s">
+      <c r="BD1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="BD1" s="3" t="s">
+      <c r="BE1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="BE1" s="4" t="s">
+      <c r="BF1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="BF1" s="5" t="s">
+      <c r="BG1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="BG1" s="5" t="s">
+      <c r="BH1" s="5" t="s">
         <v>39</v>
       </c>
     </row>
@@ -5583,31 +5589,31 @@
           <x14:formula1>
             <xm:f>'Type list'!$A$1:$A$11</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K1048576</xm:sqref>
+          <xm:sqref>L2:L1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{220336D5-88C8-43FC-BAAF-0F62C8E76DFF}">
           <x14:formula1>
             <xm:f>'Date-Qualifier list'!$A$1:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>O2:O1048576</xm:sqref>
+          <xm:sqref>P2:P1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8D7091BA-978E-46FA-96E4-C1D3C047EB93}">
           <x14:formula1>
             <xm:f>'Digital-Origin list'!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>AB2:AB1048576</xm:sqref>
+          <xm:sqref>AC2:AC1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0775DFD4-8502-4F27-ACAE-32EBE7E704B0}">
           <x14:formula1>
             <xm:f>'Capture-Device list'!$A$1:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>AE2:AE1048576</xm:sqref>
+          <xm:sqref>AF2:AF1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D7E804B7-7CD0-4C17-8008-E4590082DA8A}">
           <x14:formula1>
             <xm:f>'Continent list'!$A$1:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>AO2:AO1048576</xm:sqref>
+          <xm:sqref>AP2:AP1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>